<commit_message>
Push TC005 changes -
</commit_message>
<xml_diff>
--- a/ProjectUsingPOM/TestData/LoginData_Salesforce.xlsx
+++ b/ProjectUsingPOM/TestData/LoginData_Salesforce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHANDRASEKHARJANGA\git\RobotProject\ProjectUsingPOM\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378C4ACE-44E2-4B83-ABAA-F53EE6EAB32F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA50B1E1-0C7A-4A63-8213-51F70CE05488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{468491BC-B9C9-4F12-AC45-82C45B55A2E4}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>